<commit_message>
Se agrego complijidad de los metodos de la clase de BinomioDeNewton al excel. En la clase BinomioDeNewton se cambio el nombre del metodo obtenerBinomio a obtenerPolinomio.
</commit_message>
<xml_diff>
--- a/TP2/Complejidad.xlsx
+++ b/TP2/Complejidad.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>evaluarMSucesivas</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Ejercicio</t>
+  </si>
+  <si>
+    <t>obtenerCoeficiente</t>
+  </si>
+  <si>
+    <t>obtenerPolinomio</t>
   </si>
 </sst>
 </file>
@@ -121,15 +127,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,7 +441,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B9" sqref="B8:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,7 +462,7 @@
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -463,7 +470,7 @@
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -471,7 +478,7 @@
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -479,7 +486,7 @@
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -487,7 +494,7 @@
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -495,17 +502,25 @@
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="5"/>
+      <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>